<commit_message>
re-ran code, worked on ULs, EFSA vals
</commit_message>
<xml_diff>
--- a/tables/TableS4_country_key.xlsx
+++ b/tables/TableS4_country_key.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrition/subnational_nutrient_distributions/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7B3B2E9-ACCF-CB48-8C26-6EC32817BC17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB101B10-3900-6448-931D-EEA5F8B0C340}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="440" yWindow="1000" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableS4_country_key" sheetId="1" r:id="rId1"/>
@@ -22,27 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="68">
   <si>
-    <t>continent</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>iso3</t>
-  </si>
-  <si>
-    <t>hdi</t>
-  </si>
-  <si>
-    <t>hdi_catg</t>
-  </si>
-  <si>
-    <t>iron_type</t>
-  </si>
-  <si>
-    <t>zinc_type</t>
-  </si>
-  <si>
     <t>Africa</t>
   </si>
   <si>
@@ -224,12 +203,33 @@
   </si>
   <si>
     <t>SWE</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Zinc</t>
+  </si>
+  <si>
+    <t>HDI</t>
+  </si>
+  <si>
+    <t>HDI Category</t>
+  </si>
+  <si>
+    <t>ISO3</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Continent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -547,7 +547,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -662,6 +662,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -707,8 +718,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1063,568 +1076,578 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G1048576"/>
+      <selection activeCell="G24" sqref="A1:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2">
         <v>0.45200000000000001</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
       </c>
       <c r="D3">
         <v>0.48499999999999999</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>0.60099999999999998</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>0.54400000000000004</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>0.58399999999999996</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>0.76500000000000001</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
       </c>
       <c r="D8">
         <v>0.92900000000000005</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D9">
         <v>0.77900000000000003</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>0.92600000000000005</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>0.63200000000000001</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>0.76100000000000001</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D13">
         <v>0.61299999999999999</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D14">
         <v>0.71799999999999997</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D15">
         <v>0.93100000000000005</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D16">
         <v>0.78</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D17">
         <v>0.81599999999999995</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D18">
         <v>0.94</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D19">
         <v>0.89200000000000002</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D20">
         <v>0.89200000000000002</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D21">
         <v>0.94399999999999995</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D22">
         <v>0.86399999999999999</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D23">
         <v>0.82799999999999996</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D24">
         <v>0.94499999999999995</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>